<commit_message>
changed filter to nan instead of -1
</commit_message>
<xml_diff>
--- a/output_final.xlsx
+++ b/output_final.xlsx
@@ -1535,9 +1535,6 @@
       <c r="Z11">
         <v>22</v>
       </c>
-      <c r="AA11">
-        <v>-1</v>
-      </c>
     </row>
     <row r="12" spans="1:27">
       <c r="A12" s="1">
@@ -4440,9 +4437,6 @@
       <c r="Z46">
         <v>43</v>
       </c>
-      <c r="AA46">
-        <v>-1</v>
-      </c>
     </row>
     <row r="47" spans="1:27">
       <c r="A47" s="1">
@@ -4523,9 +4517,6 @@
       <c r="Z47">
         <v>43</v>
       </c>
-      <c r="AA47">
-        <v>-1</v>
-      </c>
     </row>
     <row r="48" spans="1:27">
       <c r="A48" s="1">
@@ -11495,9 +11486,6 @@
       <c r="Z131">
         <v>28</v>
       </c>
-      <c r="AA131">
-        <v>-1</v>
-      </c>
     </row>
     <row r="132" spans="1:27">
       <c r="A132" s="1">
@@ -18218,9 +18206,6 @@
       <c r="Z212">
         <v>27</v>
       </c>
-      <c r="AA212">
-        <v>-1</v>
-      </c>
     </row>
     <row r="213" spans="1:27">
       <c r="A213" s="1">
@@ -18301,9 +18286,6 @@
       <c r="Z213">
         <v>25</v>
       </c>
-      <c r="AA213">
-        <v>-1</v>
-      </c>
     </row>
     <row r="214" spans="1:27">
       <c r="A214" s="1">
@@ -19297,9 +19279,6 @@
       <c r="Z225">
         <v>27</v>
       </c>
-      <c r="AA225">
-        <v>-1</v>
-      </c>
     </row>
     <row r="226" spans="1:27">
       <c r="A226" s="1">
@@ -19380,9 +19359,6 @@
       <c r="Z226">
         <v>25</v>
       </c>
-      <c r="AA226">
-        <v>-1</v>
-      </c>
     </row>
     <row r="227" spans="1:27">
       <c r="A227" s="1">
@@ -20376,9 +20352,6 @@
       <c r="Z238">
         <v>27</v>
       </c>
-      <c r="AA238">
-        <v>-1</v>
-      </c>
     </row>
     <row r="239" spans="1:27">
       <c r="A239" s="1">
@@ -20458,9 +20431,6 @@
       </c>
       <c r="Z239">
         <v>25</v>
-      </c>
-      <c r="AA239">
-        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
better solution and one liner solution
</commit_message>
<xml_diff>
--- a/output_final.xlsx
+++ b/output_final.xlsx
@@ -1535,6 +1535,9 @@
       <c r="Z11">
         <v>22</v>
       </c>
+      <c r="AA11">
+        <v>17859.16666666667</v>
+      </c>
     </row>
     <row r="12" spans="1:27">
       <c r="A12" s="1">
@@ -4437,6 +4440,9 @@
       <c r="Z46">
         <v>43</v>
       </c>
+      <c r="AA46">
+        <v>8916.5</v>
+      </c>
     </row>
     <row r="47" spans="1:27">
       <c r="A47" s="1">
@@ -4517,6 +4523,9 @@
       <c r="Z47">
         <v>43</v>
       </c>
+      <c r="AA47">
+        <v>8916.5</v>
+      </c>
     </row>
     <row r="48" spans="1:27">
       <c r="A48" s="1">
@@ -11486,6 +11495,9 @@
       <c r="Z131">
         <v>28</v>
       </c>
+      <c r="AA131">
+        <v>31400.5</v>
+      </c>
     </row>
     <row r="132" spans="1:27">
       <c r="A132" s="1">
@@ -18206,6 +18218,9 @@
       <c r="Z212">
         <v>27</v>
       </c>
+      <c r="AA212">
+        <v>19709.07894736842</v>
+      </c>
     </row>
     <row r="213" spans="1:27">
       <c r="A213" s="1">
@@ -18286,6 +18301,9 @@
       <c r="Z213">
         <v>25</v>
       </c>
+      <c r="AA213">
+        <v>19709.07894736842</v>
+      </c>
     </row>
     <row r="214" spans="1:27">
       <c r="A214" s="1">
@@ -19279,6 +19297,9 @@
       <c r="Z225">
         <v>27</v>
       </c>
+      <c r="AA225">
+        <v>19709.07894736842</v>
+      </c>
     </row>
     <row r="226" spans="1:27">
       <c r="A226" s="1">
@@ -19359,6 +19380,9 @@
       <c r="Z226">
         <v>25</v>
       </c>
+      <c r="AA226">
+        <v>19709.07894736842</v>
+      </c>
     </row>
     <row r="227" spans="1:27">
       <c r="A227" s="1">
@@ -20352,6 +20376,9 @@
       <c r="Z238">
         <v>27</v>
       </c>
+      <c r="AA238">
+        <v>19709.07894736842</v>
+      </c>
     </row>
     <row r="239" spans="1:27">
       <c r="A239" s="1">
@@ -20431,6 +20458,9 @@
       </c>
       <c r="Z239">
         <v>25</v>
+      </c>
+      <c r="AA239">
+        <v>19709.07894736842</v>
       </c>
     </row>
   </sheetData>

</xml_diff>